<commit_message>
It can now print
</commit_message>
<xml_diff>
--- a/LoreHold_Legacies.xlsx
+++ b/LoreHold_Legacies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a053b728b7f22d2b/Desktop/FinalBojPRoj/ObjFinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BB859F8-66DD-4F24-876D-12F387C996E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09231075-0B03-4B30-AD43-60BA48FD3FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A19FD80C-CF95-4DB3-8536-3A2BAB30FEFA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Card ability</t>
   </si>
   <si>
-    <t>Osgiv, the Rconstructor</t>
-  </si>
-  <si>
-    <t>4 one red and white</t>
-  </si>
-  <si>
     <t>Legendary Creature - Giant Artificer</t>
   </si>
   <si>
@@ -65,7 +59,127 @@
     <t>Toughness</t>
   </si>
   <si>
-    <t xml:space="preserve">Vigilance, Cost 1 and Sacrifice and artifiact: Target creature yo ucontrol gets +2/+0 until the end of turn. Cost x and tap, Excile an artifact card with mana value X from your graveyard: Create two tokens that are copies of the exiled card. Activate only as a sorcery </t>
+    <t>Dispeller's Capsule</t>
+  </si>
+  <si>
+    <t>1 White</t>
+  </si>
+  <si>
+    <t>Artifact</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Mycosynth Wellspring</t>
+  </si>
+  <si>
+    <t>2 any</t>
+  </si>
+  <si>
+    <t>Bronze Guardian</t>
+  </si>
+  <si>
+    <t>Artifact Creature - Golem</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Steel Hellkite</t>
+  </si>
+  <si>
+    <t>6 any</t>
+  </si>
+  <si>
+    <t>Angle of the Ruins</t>
+  </si>
+  <si>
+    <t>Artifact Creature - Dragon</t>
+  </si>
+  <si>
+    <t>Artifact Creatrue - Angle</t>
+  </si>
+  <si>
+    <t>Cursed Mirror</t>
+  </si>
+  <si>
+    <t>Monologue Tax</t>
+  </si>
+  <si>
+    <t>Enchantment</t>
+  </si>
+  <si>
+    <t>Ledendary Planeswalker - Daretti</t>
+  </si>
+  <si>
+    <t>Boros Locket</t>
+  </si>
+  <si>
+    <t>Secret Rendezvous</t>
+  </si>
+  <si>
+    <t>Sorcery</t>
+  </si>
+  <si>
+    <t>You and target opponent each draw three cards</t>
+  </si>
+  <si>
+    <t>Osgiv; the Rconstructor</t>
+  </si>
+  <si>
+    <t>4 any; 1 Red and White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vigilance; Cost 1 and Sacrifice and artifiact: Target creature yo ucontrol gets +2/+0 until the end of turn. Cost x and tap; Excile an artifact card with mana value X from your graveyard: Create two tokens that are copies of the exiled card. Activate only as a sorcery </t>
+  </si>
+  <si>
+    <t>2 any and 1 white and tap; Sacrifice Dispeller's Capsule: Destroy target artifact or enchantment.</t>
+  </si>
+  <si>
+    <t>When Mycosynth Wellspring enters the battlefield or is put inot a graveyard from the battlefield; you may search your library for a basic land card; reveal it; put it into your hand; then shuffle.</t>
+  </si>
+  <si>
+    <t>4 any; 1 White</t>
+  </si>
+  <si>
+    <t>Double strike; Ward 2; Other artifacts you control have ward 2. Bronze Guardian's power is equal to the number of artifacts you control.</t>
+  </si>
+  <si>
+    <t>Flying; 2 any: Steel Hellkite gets +1/+0 until the end of turn. X any: Destroy each nonland permanent with mana value X whose controller was dealt comabt damage by Steel Hellkite this turn. Activate only once each turn.</t>
+  </si>
+  <si>
+    <t>5 any; 2 White</t>
+  </si>
+  <si>
+    <t>Flying; When Angel of the Ruins enters the battlefield; exile up to two target artifacts and/or enchantments. Plainscycleing: 2 Any (Discard this card: Search your library for a plains card; reveal it;put it into your hand; then shuffle.)</t>
+  </si>
+  <si>
+    <t>2 Any; 1 Red</t>
+  </si>
+  <si>
+    <t>tap: Add 1 Red. As Cursed Mirror enters the battlefield; you may have it become a copy of any creature on the battlefield until end of turn; except it has haste.</t>
+  </si>
+  <si>
+    <t>2 Any; 1 White</t>
+  </si>
+  <si>
+    <t>Whenever an opponent casts their second spell each turn; you create a Treasure token.</t>
+  </si>
+  <si>
+    <t>Daretti; Scrap Savant</t>
+  </si>
+  <si>
+    <t>3 Any; 1 Red</t>
+  </si>
+  <si>
+    <t>|+2 toughness: Discart up to two cards; then draw that many cards. -2: Sacrifice an artifact. If you do; return target artifact card from your graveyard to the battlefeild. -10: You get an emblem with "Whenever an artifact is put into your graveyard from the battlefield; return that card to the battlefield at the beginning of the next end step." Daretti; Scrap Savant can be your commander.C13</t>
+  </si>
+  <si>
+    <t>tap: Add 1 Red and 1 White. 4 Red or White; tap Scarifice Boros Locket: Draw two cards.</t>
+  </si>
+  <si>
+    <t>1 Any; 2 White</t>
   </si>
 </sst>
 </file>
@@ -118,6 +232,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DA36E9-54C7-4D89-9BFD-8078D5131E6D}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,30 +564,230 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>4</v>
       </c>
       <c r="F2">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>